<commit_message>
2021-0421 檢查 Excel Block 完成
</commit_message>
<xml_diff>
--- a/R2/2021-0421 檢查 Excel Block/RCAD-鋼筋型文對照表-圖塊SigoAva-Mu-MEI-AVA-20210412-鋼筋計料.xlsx
+++ b/R2/2021-0421 檢查 Excel Block/RCAD-鋼筋型文對照表-圖塊SigoAva-Mu-MEI-AVA-20210412-鋼筋計料.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\autohotkey\R2\2021-0421 檢查 Excel Block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52861317-0378-4D16-9DA3-D97832066E50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA74A0-78A1-442D-844B-22384D3085EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="3225" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,7 +805,7 @@
         <xdr:cNvPr id="2" name="直線接點 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A7850D0-0D02-46D0-A854-31FB2616874A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E17834D-3A48-4C89-AE23-D459C22A14E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -860,7 +860,7 @@
         <xdr:cNvPr id="3" name="直線接點 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B033C20E-1200-4140-8FD4-F36ADB96BD8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D07A9B-BEBB-4015-B09E-9182DD8D4AA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -915,7 +915,7 @@
         <xdr:cNvPr id="4" name="直線接點 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1EE91C9-4A6D-472C-B054-DBA5E08C65D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0625C460-0AA7-4C5D-9EF1-BB889C866047}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -970,7 +970,7 @@
         <xdr:cNvPr id="5" name="直線接點 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDF118E1-51B9-4C3C-8A81-D03C1509E100}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45EEA085-65A5-461D-9599-19119174789A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,7 +1025,7 @@
         <xdr:cNvPr id="6" name="直線接點 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFEF6399-8DD7-46EF-B04F-9D0AA90CD696}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69F21882-7D74-4A43-B80D-989D3BF91265}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1080,7 +1080,7 @@
         <xdr:cNvPr id="7" name="直線接點 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EAD42EA-7413-4065-AF56-FD38390B39D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{621DDF31-6B6C-4B6A-A70A-0355DC076220}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1135,7 +1135,7 @@
         <xdr:cNvPr id="8" name="直線接點 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1420C4-660D-487C-8F9B-7E67B8FB6BEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0310168E-0939-444A-A7FC-1A999702947E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1190,7 +1190,7 @@
         <xdr:cNvPr id="9" name="直線接點 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9FD770D-42DC-4247-8526-10DD71965F2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8785742D-EDCC-4B84-BC42-FB9404594603}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1245,7 +1245,7 @@
         <xdr:cNvPr id="10" name="文字方塊 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF34097F-CA14-4EFE-9217-0285EE60EABD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35DCE3F-4B60-46E5-B014-A48A92C0418C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1343,7 @@
         <xdr:cNvPr id="11" name="文字方塊 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60A255FE-8081-471B-994E-D21514FEAB97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126C3CE9-790B-4AB3-9406-405985EC69EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1441,7 +1441,7 @@
         <xdr:cNvPr id="12" name="直線接點 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236417A7-4828-4A9C-9793-548D4E4E88F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A07F197-6A1C-4656-92A7-BDCCF95A2860}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1496,7 +1496,7 @@
         <xdr:cNvPr id="13" name="直線接點 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E3A8FC-561B-4C7B-8EFA-C2DC5A3ACA44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E5FFE38-8E4A-49EE-A50D-019BE2A6C857}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1551,7 +1551,7 @@
         <xdr:cNvPr id="14" name="直線接點 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B00A12B-CCE3-413D-BC5F-2F4B7D2EB0C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FEDEC80-384E-421B-9FF7-2407C6CD5B60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1606,7 +1606,7 @@
         <xdr:cNvPr id="15" name="直線接點 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B322201-B4B5-4DEC-84D0-5F5D2586983E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58D56BA2-1385-41C4-BA62-AAAEAF02DD39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1661,7 +1661,7 @@
         <xdr:cNvPr id="16" name="直線接點 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4972F580-0A98-4A32-AF76-EAD8C9F81A83}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{159EF9D8-9F2E-4B4F-A7D6-1B2DEC1C9D49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1716,7 +1716,7 @@
         <xdr:cNvPr id="17" name="文字方塊 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EFA0AB6-31E1-4B23-A2A4-67F83FC5A0F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{720C36DD-2D0C-45BD-B951-84AFBA933361}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1814,7 +1814,7 @@
         <xdr:cNvPr id="18" name="文字方塊 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93C4C9B2-E284-424A-BA54-F77E2FB94939}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C27DDD5-DA06-4EBB-9B76-DB9C12D90F2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1912,7 +1912,7 @@
         <xdr:cNvPr id="19" name="直線接點 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD2AA6D1-A030-4C2A-A228-8C4CA0361550}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{229A26A0-D9BE-4FAE-8825-1824D27ED897}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1967,7 +1967,7 @@
         <xdr:cNvPr id="20" name="直線接點 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5354B85E-72D0-4837-8C28-D001EE6BEBF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B2C9C5E-0A5C-404F-8FC0-56364772A538}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2022,7 +2022,7 @@
         <xdr:cNvPr id="21" name="文字方塊 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F19B6FFF-4ECA-409D-BEAB-E662D6500944}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FDC4F0E-EDB3-4C84-9581-066B39790E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2120,7 +2120,7 @@
         <xdr:cNvPr id="22" name="直線接點 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53CCDE01-F0AA-4418-B6D2-7CACEEA831D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D8A4D3-AABB-43F4-9057-E5EE7B44DEB6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2175,7 +2175,7 @@
         <xdr:cNvPr id="23" name="直線接點 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C47853-CA12-4391-871C-D61925509EDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28528B9C-1095-4CEE-A46C-72B3C4B2A2E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2230,7 +2230,7 @@
         <xdr:cNvPr id="24" name="直線接點 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E024EF5-884F-4F8D-A6EC-9E7D390AD5BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ACB7F24-55D4-4040-92A2-8F3AA5236251}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2285,7 +2285,7 @@
         <xdr:cNvPr id="25" name="直線接點 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E5C931-2E73-4485-A5B6-47EDD8665482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9406E678-A886-4C14-8F03-BA2CE04BE39E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2340,7 +2340,7 @@
         <xdr:cNvPr id="26" name="直線接點 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F570DF4-F633-4DA2-BE56-EEC10A6FC466}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AED8019-565E-49C7-A862-70AE2E1A9FA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2395,7 +2395,7 @@
         <xdr:cNvPr id="27" name="直線接點 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087F33EF-EB36-48F6-8A6F-1566C67141AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F64A7F-DDAA-42EF-B817-727DAFF8231F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2450,7 +2450,7 @@
         <xdr:cNvPr id="28" name="直線接點 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5F2EC8-1716-497E-AC53-0BACF523FDFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D512E69D-86BB-42FD-8CE1-EAA4BADD888B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2505,7 +2505,7 @@
         <xdr:cNvPr id="29" name="直線接點 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64BAB17A-6884-424D-BF09-A55CA191C63A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96DA5C75-1CCC-4D13-BA67-98C3102772FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2560,7 +2560,7 @@
         <xdr:cNvPr id="30" name="直線接點 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A2DFA9-58FC-457A-BB84-93DF6CB2E458}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF5FF4F-F237-479C-8E18-247A253FE73F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2615,7 +2615,7 @@
         <xdr:cNvPr id="31" name="直線接點 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2330F126-F709-41CF-86F0-39709D574862}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D1C155-D8D4-43D4-BD1E-53ABC58F619A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2670,7 +2670,7 @@
         <xdr:cNvPr id="32" name="直線接點 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F5D3E17-9CAE-4F4E-9F80-5CB8BD1229C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3387FC82-C604-4BBF-A160-1F5CBF9A4E90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2725,7 +2725,7 @@
         <xdr:cNvPr id="33" name="直線接點 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{374C4B44-CBAB-4AC0-AE26-19434E29236B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82886488-BEDB-44B3-9A4F-360069D3BA6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2780,7 +2780,7 @@
         <xdr:cNvPr id="34" name="文字方塊 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BDDD7C9-F8ED-4D05-B2DC-9B6465585581}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C2E202-FDFA-4F58-A0BB-7354BA0CB234}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2878,7 +2878,7 @@
         <xdr:cNvPr id="35" name="文字方塊 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B848D64-2CAE-4563-B8ED-0D9DF585B8BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5559A0F-038B-4D03-88E8-0898AE88B994}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2976,7 +2976,7 @@
         <xdr:cNvPr id="36" name="文字方塊 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A6D45BF-3728-49F4-93F1-4207A2790325}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E33BBFD3-5580-4BF9-89C6-39AA7D830CDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3074,7 +3074,7 @@
         <xdr:cNvPr id="37" name="直線接點 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525BE52F-1B54-4821-9E7A-2A03CAF5C0BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DE16CE-8300-49D2-9110-0F9E3DC978B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,7 +3129,7 @@
         <xdr:cNvPr id="38" name="直線接點 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B8394B0-D72D-41D6-A53F-A4BE64E886C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{683EB015-4722-4BB2-BB0B-4644A09EF82A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3184,7 +3184,7 @@
         <xdr:cNvPr id="39" name="直線接點 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FFFA705-5D4C-4F37-A33C-A30F58C329BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4360F02B-F954-4DCC-A3E2-50A87D30CB4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3239,7 +3239,7 @@
         <xdr:cNvPr id="40" name="直線接點 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465044D1-A49D-4AA8-98FB-DB6EE7584B59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58A8728-AEA6-45A6-ACEB-730F6405D611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3294,7 +3294,7 @@
         <xdr:cNvPr id="41" name="直線接點 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C44C49D7-C9E7-4933-9CB2-29B6D2C726FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06008D4E-E082-4E37-ABE3-2C4C3F817CF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3349,7 +3349,7 @@
         <xdr:cNvPr id="42" name="直線接點 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70584F67-B1C9-4908-A55E-28748AFC2633}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA5C31D-2AA6-4FDB-B86A-D48DCD0B931A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3404,7 +3404,7 @@
         <xdr:cNvPr id="43" name="直線接點 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BF7BD24-6AC0-4741-BDB4-EDD194F3C7CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EBDB877-E1D8-484E-8319-C9FF28B869A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3459,7 +3459,7 @@
         <xdr:cNvPr id="44" name="直線接點 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F70B550B-4544-4EFF-8684-73FA6C02B599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32F1240-05C6-43F3-8E83-9CC5A298ACAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3514,7 +3514,7 @@
         <xdr:cNvPr id="45" name="直線接點 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40905548-FB63-4719-B84F-A5EF0860D7BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81F36D7C-C863-4FB0-B4B1-34B7E2AEA225}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3569,7 +3569,7 @@
         <xdr:cNvPr id="46" name="直線接點 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF964904-4047-4D07-938C-341EB38C8A04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F736EF43-6D0C-4C29-9C67-4A3432206A0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3624,7 +3624,7 @@
         <xdr:cNvPr id="47" name="直線接點 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FBA0BEA-89DD-4471-8766-3F26D2321B25}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AC99C0-1829-4197-903C-0DCF5641D883}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3679,7 +3679,7 @@
         <xdr:cNvPr id="48" name="直線接點 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EDF575F-2BC9-44BE-8286-07EE3E9ABCD8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EFC8B5F-8B74-44E3-BC26-DA88026A847C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3734,7 +3734,7 @@
         <xdr:cNvPr id="49" name="文字方塊 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E460E7-54A7-4439-A8BC-1C9CB8E16237}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B018BF4D-571B-4F77-ABFC-FC1BB1F96CA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3832,7 +3832,7 @@
         <xdr:cNvPr id="50" name="文字方塊 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A84518E-B087-4033-A724-45BFBC837434}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19E507E5-0364-4034-9BFF-0EC8336CAD22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3930,7 +3930,7 @@
         <xdr:cNvPr id="51" name="文字方塊 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A08E2C07-C154-46D6-9D4B-B29630FF4809}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F88113-7575-4D0D-9F3B-9CA1AE62E553}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4028,7 +4028,7 @@
         <xdr:cNvPr id="52" name="直線接點 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E0C5A3-A2D9-41F6-9455-99BA4D88094C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B38890-3737-4CC2-955E-DD57E9A30C83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4083,7 +4083,7 @@
         <xdr:cNvPr id="53" name="直線接點 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94DD3C30-2A24-464A-81D1-CCF4B9655F32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788C8A44-C83E-4C3E-9922-A90319FEA830}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4138,7 +4138,7 @@
         <xdr:cNvPr id="54" name="直線接點 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{357A2584-C239-4A09-AC5B-B0F341B73FCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EBBA540-7A81-4518-B840-D9C4A4781609}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4193,7 +4193,7 @@
         <xdr:cNvPr id="55" name="直線接點 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1652C78D-3B75-4BB6-821A-307C5F944E50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBB4836-0E26-491F-80C2-50CF693B0D45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4248,7 +4248,7 @@
         <xdr:cNvPr id="56" name="直線接點 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944FA9CF-18AE-4150-A2B8-9A98F9420247}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCC606-50D6-41C3-9641-B4BEEE362777}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4303,7 +4303,7 @@
         <xdr:cNvPr id="57" name="直線接點 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BAD9078-DA67-44AB-B1F3-0558D76E154F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{437C3867-6579-4BAE-B287-E8B30AED4D03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4358,7 +4358,7 @@
         <xdr:cNvPr id="58" name="直線接點 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D65C396B-385F-4A4C-B61B-41AB1D392C1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DD0A53E-6221-45B1-B9B1-B809F061ACFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4413,7 +4413,7 @@
         <xdr:cNvPr id="59" name="直線接點 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD0FF77D-0F76-4EB8-A57F-DF33C82F20C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{950D7C53-3DEE-4C8F-8CB2-F218A7F25861}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4468,7 +4468,7 @@
         <xdr:cNvPr id="60" name="直線接點 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60A22A92-ADA8-4089-A1B7-34FC42252D4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5DF8048-BF5E-4C4A-B521-9D2C91C35399}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4523,7 +4523,7 @@
         <xdr:cNvPr id="61" name="文字方塊 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB56CF16-719A-4686-9416-23EE54236C58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C2A6F8-4397-47B2-96FC-F0B91EADF8C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4621,7 +4621,7 @@
         <xdr:cNvPr id="62" name="文字方塊 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAED11BD-2ECB-436C-8768-9467315658F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69BED8BD-4713-4BAA-B67A-17D1FC8226A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4719,7 +4719,7 @@
         <xdr:cNvPr id="63" name="文字方塊 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004E657A-46CC-43DF-AFDF-160F21562504}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F958F28-8CA4-48E5-B063-8F2EDA2B8599}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4817,7 +4817,7 @@
         <xdr:cNvPr id="64" name="直線接點 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00685EC6-7BD7-4D69-92DF-02D235DE8760}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC4185B-DE74-4B98-B58A-11CDDC042851}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4872,7 +4872,7 @@
         <xdr:cNvPr id="65" name="直線接點 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708C7FEC-60ED-46F7-B314-449722B3C2B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC5E898-29A5-4647-9E01-1B760D3305D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4927,7 +4927,7 @@
         <xdr:cNvPr id="66" name="直線接點 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B7BAEE-1971-48BB-A535-21167BE6A4C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB75856D-3B1B-4ECF-B40E-9963203A2AF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4982,7 +4982,7 @@
         <xdr:cNvPr id="67" name="直線接點 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB51DD26-21C4-41F9-8710-AABE58571346}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2317DCEF-28D2-415C-9B05-2D8C8ED79DB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5037,7 +5037,7 @@
         <xdr:cNvPr id="68" name="直線接點 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F5A1420-D6B4-4C19-935D-E6DD0F5D6594}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{065EDF13-50C0-4EE5-B09B-E5C5314384E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5092,7 +5092,7 @@
         <xdr:cNvPr id="69" name="直線接點 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433499F1-53D4-42EB-8311-03DBC54849C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12009B26-59F8-420A-A967-60B3244BF641}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5147,7 +5147,7 @@
         <xdr:cNvPr id="70" name="文字方塊 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEF31C53-22BE-4CC5-8A47-A96969809FB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{051FEB6E-B5A2-46A2-B42F-2FD85995CAD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5245,7 +5245,7 @@
         <xdr:cNvPr id="71" name="文字方塊 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{305A674D-92B7-4788-A715-C54D2942D9B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64F13586-0C2F-4246-AE27-CF96FDE57575}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5343,7 +5343,7 @@
         <xdr:cNvPr id="72" name="文字方塊 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD05E3B2-CA01-4670-81F0-896ACAF68451}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAFE27E1-170D-4B44-86DC-AB376BF2D3F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5441,7 +5441,7 @@
         <xdr:cNvPr id="73" name="直線接點 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF0F6CDD-E988-4B51-9348-3110489CE39D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8720ACAE-85A3-42C0-BDE7-21089F3636C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5496,7 +5496,7 @@
         <xdr:cNvPr id="74" name="直線接點 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86C323BB-37FF-424D-92B3-CF41083E8482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EFF567B-390C-4442-A8E4-2C5280C415D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5551,7 +5551,7 @@
         <xdr:cNvPr id="75" name="直線接點 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD999867-81DA-4B05-A566-C5FA57D8DC78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86A79804-D651-4D8B-A6AF-F64EB19EAA71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5606,7 +5606,7 @@
         <xdr:cNvPr id="76" name="直線接點 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9F4842A-139E-4763-9D57-1E8A2FFD896C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B87402F-09F5-4607-BA6C-2677698AEE12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5661,7 +5661,7 @@
         <xdr:cNvPr id="77" name="直線接點 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F60B0B72-6675-42CC-B572-599759962ED0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB1C0EA0-F463-42C1-AB86-22DA9C4362BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5716,7 +5716,7 @@
         <xdr:cNvPr id="78" name="直線接點 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F8E92B-C284-40EA-9512-0E2FDB4E417A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{198D83A2-303C-43E4-86E9-78DACE5FC48E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5771,7 +5771,7 @@
         <xdr:cNvPr id="79" name="文字方塊 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3334B613-34DA-4E62-99F4-FAF350E83BF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7B9C927-7D2A-4B56-B2A4-311285A75EB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5869,7 +5869,7 @@
         <xdr:cNvPr id="80" name="文字方塊 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{208C7A3C-ADD1-4A55-A3C6-5984894AE64A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9E8842-6145-4BA9-92BC-10C9CED460CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5967,7 +5967,7 @@
         <xdr:cNvPr id="81" name="直線接點 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A212D191-E8F3-4C88-B886-D935B0D898EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F725517-733F-412A-838B-061ABCA3A5EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6022,7 +6022,7 @@
         <xdr:cNvPr id="82" name="直線接點 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{923D32D6-92BA-4832-8BEC-4C8BB6393CEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{123B88BB-72D8-4BA5-9402-AFDD6CC66875}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6077,7 +6077,7 @@
         <xdr:cNvPr id="83" name="直線接點 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{047B4012-C401-4129-A4B1-A8CC94EB8035}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A07B2B53-156A-4CBD-A169-720A9ECFBA8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6132,7 +6132,7 @@
         <xdr:cNvPr id="84" name="直線接點 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1604620-A9A4-48D1-9050-7E608F31BA6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B4AF94-BAD0-48FA-A3FD-E511AA9622A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6187,7 +6187,7 @@
         <xdr:cNvPr id="85" name="直線接點 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB551286-C3B7-425E-8249-772BAA56CAEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93615921-979C-4434-A6CE-0CBDBE4B3A72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6242,7 +6242,7 @@
         <xdr:cNvPr id="86" name="直線接點 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1523A1B8-8532-4E2D-BABF-08A47A152DC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B59E38A-9151-4715-8ACE-224EE4CC201D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6297,7 +6297,7 @@
         <xdr:cNvPr id="87" name="直線接點 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBDCD587-6CAA-4D12-A52E-A109A8F01A3F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42EEDD2E-CBD1-431C-9594-B41B97F8C234}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6352,7 +6352,7 @@
         <xdr:cNvPr id="88" name="直線接點 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{492CEC2B-7506-4AA9-9A1E-CCFBC207A8CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546FBA36-0C56-48C6-8C49-D54CEFDDB4C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6407,7 +6407,7 @@
         <xdr:cNvPr id="89" name="直線接點 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{050D5530-4EDE-43B7-9DF3-1FA05A24D057}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249ACAE0-13D3-4AF8-B449-C049CE89B3F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6462,7 +6462,7 @@
         <xdr:cNvPr id="90" name="直線接點 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558E2B59-0554-4356-9510-C3B879DAF821}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30311D45-9F1C-44D5-8E87-275D4278B4EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6517,7 +6517,7 @@
         <xdr:cNvPr id="91" name="直線接點 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C93A6E5B-349C-4B59-B6CC-F0A257994CC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2941B64-BE64-4BBE-884C-A2A61E654A8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6572,7 +6572,7 @@
         <xdr:cNvPr id="92" name="直線接點 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB36890A-73E5-4577-AF42-397B3B6DFCEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{277F4E4C-84AF-4FF7-A5E8-3AF13A11645B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6627,7 +6627,7 @@
         <xdr:cNvPr id="93" name="直線接點 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DD39A1F-1E94-41BC-8D16-54B24888ADBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938E580B-138D-40A2-8D5A-CD4E0628131D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6682,7 +6682,7 @@
         <xdr:cNvPr id="94" name="直線接點 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6CDE330-6403-4541-B9DC-C32F056A954E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D369768-0F98-4826-8778-CBB734D01055}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6737,7 +6737,7 @@
         <xdr:cNvPr id="95" name="直線接點 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ECA3586-C4A8-4356-8470-BE7C0E4BCCA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6B9725D-220C-4BFB-8352-DD2C5F41067F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6792,7 +6792,7 @@
         <xdr:cNvPr id="96" name="文字方塊 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B1F9A23-F409-4CF4-BA77-AE11CA74054F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4302D60-79E0-406A-87C8-05020D9B0C55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6890,7 +6890,7 @@
         <xdr:cNvPr id="97" name="文字方塊 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D1DD06-44E9-43E1-A024-2D483CE067BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F9AB9EF-34B1-4B55-A97A-46BA51F6E2B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6988,7 +6988,7 @@
         <xdr:cNvPr id="98" name="文字方塊 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6813318E-ED51-42E9-A6A0-005669078D7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EED37909-03C6-42E4-B21B-00EC427B2A43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7086,7 +7086,7 @@
         <xdr:cNvPr id="99" name="直線接點 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3EF4A58-DD16-40BC-8735-66E610888789}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1070240-0917-4651-A6D0-C9503529990C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7141,7 +7141,7 @@
         <xdr:cNvPr id="100" name="直線接點 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AE625C4-284D-4B37-8A4C-5C55B17C5243}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963E42F7-FE93-4177-82E2-601910F7A7BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7196,7 +7196,7 @@
         <xdr:cNvPr id="101" name="直線接點 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B16E41-6C62-4933-B9F6-8B0367C8F057}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE3CF8C-837A-44B8-9BF8-779EBFF4C728}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7251,7 +7251,7 @@
         <xdr:cNvPr id="102" name="直線接點 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A9F4F1-00D0-449B-8A9C-4803FADECA3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77034E85-F30B-4B5B-B315-CAA3832F656B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7306,7 +7306,7 @@
         <xdr:cNvPr id="103" name="直線接點 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A491B46-783D-47A3-9258-4A3678EBDFB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87BDC8C0-EC0E-4BA9-8AED-0940754CDECA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7361,7 +7361,7 @@
         <xdr:cNvPr id="104" name="直線接點 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F36AF1AF-F872-457B-99CB-E8841F47AED7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67F4CDA2-0DA9-47A7-986D-7EEA42781D25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7416,7 +7416,7 @@
         <xdr:cNvPr id="105" name="直線接點 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C1761B-D05E-447A-8CF1-D82A28B2DAD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6C8D92-236D-48F9-B7C5-70800D89A89E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7471,7 +7471,7 @@
         <xdr:cNvPr id="106" name="直線接點 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2361A0B3-9596-4203-99BC-25D0EACB7575}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA760A3F-3439-45F4-A2D8-0BB013AB5E8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7526,7 +7526,7 @@
         <xdr:cNvPr id="107" name="直線接點 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4394EBCB-5E14-43AD-9AB3-D95898B9F23A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C80F1293-7A09-4E61-8203-849C0E9CF8C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7581,7 +7581,7 @@
         <xdr:cNvPr id="108" name="文字方塊 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2219D3B5-94AA-42B1-ABEE-ED645DCF7399}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7F75232-B63E-47EB-97D1-B674234241C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7679,7 +7679,7 @@
         <xdr:cNvPr id="109" name="文字方塊 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38EB67DC-0EA1-46A6-9E02-2FCA305FAD0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFC76E4-1E9D-48FD-AA4F-267A6585B245}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7777,7 +7777,7 @@
         <xdr:cNvPr id="110" name="文字方塊 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF30E682-0ABC-4AF3-AA41-562CC8115339}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD91C9E3-6442-418C-B12A-3EB3AB01885F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7875,7 +7875,7 @@
         <xdr:cNvPr id="111" name="直線接點 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86CA2A76-DCD0-4236-91CA-B39CA3BA4439}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92177A1A-C4C2-4F1D-974D-FF0EEF62F188}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7930,7 +7930,7 @@
         <xdr:cNvPr id="112" name="直線接點 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86B4D14A-FF2B-48C2-B59E-D733022D8533}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E0DA01C-23D6-452D-A77A-F247CF14FB4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7985,7 +7985,7 @@
         <xdr:cNvPr id="113" name="直線接點 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB42B05-7530-459D-A41A-3A07C8E64524}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D1BA27-19FA-435D-B6CA-95634EFE295B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8040,7 +8040,7 @@
         <xdr:cNvPr id="114" name="文字方塊 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8AFAF1-DF7D-4B59-B713-6834CEC6C163}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D3FFB2-FCF9-46F4-94EF-1854239D03E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8138,7 +8138,7 @@
         <xdr:cNvPr id="115" name="直線接點 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A3E1F0-75C7-46E1-9A0B-B1BF9C0083D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8620B0C0-653D-4458-939A-A68858F361F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8193,7 +8193,7 @@
         <xdr:cNvPr id="116" name="直線接點 115">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E66B7E-EA8B-47A7-93D7-41B77F2B2943}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36267CCE-EA95-4A2C-AEB7-23EB920164C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8248,7 +8248,7 @@
         <xdr:cNvPr id="117" name="直線接點 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A58C4BA-1D24-4D4E-A307-B68943419178}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81ABBB30-7730-4322-924B-0696DD8AAB8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8303,7 +8303,7 @@
         <xdr:cNvPr id="118" name="直線接點 117">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCF35EE2-35CC-453F-AA44-040706626995}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31636BD4-3F3C-4488-AAB8-E8EB2810217F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8358,7 +8358,7 @@
         <xdr:cNvPr id="119" name="弧形 118">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2761D6D-01A3-4C95-906F-769965A25171}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A76F6EF4-9F20-4C94-B996-209C4854526A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8424,7 +8424,7 @@
         <xdr:cNvPr id="120" name="弧形 119">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E78FB1D-EB24-480B-B622-9127985E414C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB6F08C-16C2-41A3-A52D-72FB61147AC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8490,7 +8490,7 @@
         <xdr:cNvPr id="121" name="文字方塊 120">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB95E461-EB86-45EA-A6F4-663EB2C980FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACBB7DBA-C145-4220-80B8-1E95136778DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8588,7 +8588,7 @@
         <xdr:cNvPr id="122" name="文字方塊 121">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50062EAB-4AE5-4237-AA7D-16683484CDB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88ABA9A4-EA1A-4005-92F5-BAF047CD9AA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8686,7 +8686,7 @@
         <xdr:cNvPr id="123" name="文字方塊 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9F39F0-03F9-4DFE-A6ED-B2F434EBE3C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABECFA0F-839C-46D9-82A4-21D56CB2399D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8784,7 +8784,7 @@
         <xdr:cNvPr id="124" name="文字方塊 123">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3525CA-A5C3-4B6F-BDCB-1599BD0C2FE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41276449-7A23-441D-AE6A-CEF286C27666}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8882,7 +8882,7 @@
         <xdr:cNvPr id="125" name="直線接點 124">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AFE5970-E0DB-4915-ACAF-3C5D09D74538}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C067E544-7077-4881-A70B-1E2318193935}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8937,7 +8937,7 @@
         <xdr:cNvPr id="126" name="直線接點 125">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B541E9-BEC3-4C14-944C-0A426ECF8196}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC9FE2E3-F3EC-4D38-A84B-B613A09364B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8992,7 +8992,7 @@
         <xdr:cNvPr id="127" name="直線接點 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8D7AF8A-09A4-439C-8F96-20B10987DE86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{299A6C2D-7FBD-49A3-A70E-90A8AA8A67B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9047,7 +9047,7 @@
         <xdr:cNvPr id="128" name="直線接點 127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2548CF5D-8087-4D7A-8DB5-60852AD6D865}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898836CE-D9FD-4075-A808-0892FCC77E17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9102,7 +9102,7 @@
         <xdr:cNvPr id="129" name="直線接點 128">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F28D4BCE-03E4-4E31-8927-281EE263A1A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA197D75-3A28-4A90-B0A5-AEF3D05C7418}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9157,7 +9157,7 @@
         <xdr:cNvPr id="130" name="直線接點 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE4DC015-9D86-4CD4-A919-3771DF71BC22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478BAD33-4257-48EF-8156-D81061C217F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9212,7 +9212,7 @@
         <xdr:cNvPr id="131" name="直線接點 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B423BC6A-59A9-43A2-874E-578D08D1A150}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3068B6-20AB-4F55-A473-0D94C2899576}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9267,7 +9267,7 @@
         <xdr:cNvPr id="132" name="直線接點 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0051EF1B-4397-4260-927F-BBB6CC962FE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1080A99-536D-48F4-BBAA-1E0B9D9E3B81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9322,7 +9322,7 @@
         <xdr:cNvPr id="133" name="直線接點 132">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95D9DA8A-FAB2-40AC-82D7-6426C562CC06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5178E9BE-D4F1-4866-BF91-0DAEBA24B646}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9377,7 +9377,7 @@
         <xdr:cNvPr id="134" name="直線接點 133">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEA8F7-8BD4-48A1-8E02-886A2502BF14}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B366AA66-49E8-4395-BBD4-914EC393DD11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9432,7 +9432,7 @@
         <xdr:cNvPr id="135" name="直線接點 134">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D77B8A-B9E6-4D56-A694-7480879C6BE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91965DA7-C9ED-4EB9-A054-4D3B32ECFD7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9487,7 +9487,7 @@
         <xdr:cNvPr id="136" name="直線接點 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C82D29-D31F-4360-B7DE-209E2F4560A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14786ADE-A000-43EB-9BE0-108A12DFBAC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9542,7 +9542,7 @@
         <xdr:cNvPr id="137" name="文字方塊 136">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECE3C946-1278-4DA3-B685-4C6434D97EA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB820CF8-FBB2-4CBE-9ADF-7A5092E57672}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9640,7 +9640,7 @@
         <xdr:cNvPr id="138" name="文字方塊 137">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C170EDC-BEFE-45BC-845A-FFDB0F00D0D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E126585B-5B6D-4425-BBBF-2FCFB3C64B12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9738,7 +9738,7 @@
         <xdr:cNvPr id="139" name="文字方塊 138">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CE41849-6039-4662-8A2C-53FD6B196649}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F51FA961-A93A-4084-9C4B-AB5B9B8DBAF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9836,7 +9836,7 @@
         <xdr:cNvPr id="140" name="直線接點 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49666055-9338-4882-8802-CFFCC0F978A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82664704-6F9A-4C3D-8636-8D1734484F27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9891,7 +9891,7 @@
         <xdr:cNvPr id="141" name="直線接點 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8F85626-CE69-435E-A79F-890BA3C5F2EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7064B1E-4A38-473A-80D5-CE871DEB7A43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9946,7 +9946,7 @@
         <xdr:cNvPr id="142" name="文字方塊 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71991039-0A2A-4461-AF25-4F1C9448A28B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA8094F-030C-4F10-9456-B586411F784A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10044,7 +10044,7 @@
         <xdr:cNvPr id="143" name="文字方塊 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C784CFF-032B-4A66-92BE-FF7D9C3D614B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{520F7FFC-6309-4787-BD64-5C2445262AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10142,7 +10142,7 @@
         <xdr:cNvPr id="144" name="文字方塊 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69B00FF0-41A6-4D3F-BF24-1E356BD74C26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A879018-34A6-4C9C-B0A2-7ACE69A6A170}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10240,7 +10240,7 @@
         <xdr:cNvPr id="145" name="直線接點 144">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{551CFA1D-1B68-4049-A81D-5D8F6CBBE4AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1C757E-F4B2-4CBB-9519-E65DFB3EBB66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10295,7 +10295,7 @@
         <xdr:cNvPr id="146" name="直線接點 145">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8E72962-EDA5-4E5D-B71B-551E6305CE08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2F2CE4A-2DF1-45C6-BD6D-DB996321E7C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10350,7 +10350,7 @@
         <xdr:cNvPr id="147" name="直線接點 146">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0818161-9CBD-4B39-A520-2ABC5C9591D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CC4E48A-CF21-47C8-BE43-721E6E194689}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10405,7 +10405,7 @@
         <xdr:cNvPr id="148" name="文字方塊 147">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{149A0101-EAEA-47D7-9719-78FC6A29D7ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0760ED1D-720C-466F-BEDD-31E2DC95792F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10503,7 +10503,7 @@
         <xdr:cNvPr id="149" name="文字方塊 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF07B30F-D61A-4FE3-A71F-1E7589F785A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F16650AD-B871-401D-9B17-53E97530B534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10601,7 +10601,7 @@
         <xdr:cNvPr id="150" name="文字方塊 149">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F561B68C-4826-4A57-A273-D4A30A092928}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C023BCD4-0023-42AD-A99D-4B02A7B6A4AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10699,7 +10699,7 @@
         <xdr:cNvPr id="151" name="直線接點 150">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D2AF413-9565-458A-BF30-DA84E77A8220}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5916881-4CA6-49E7-A045-9FA254B811C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10754,7 +10754,7 @@
         <xdr:cNvPr id="152" name="直線接點 151">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35540C38-789E-48A7-B532-330C0B26B049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DBF7D5B-DABC-460B-8818-A0F52997840A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10809,7 +10809,7 @@
         <xdr:cNvPr id="153" name="直線接點 152">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD588C7-B972-4925-991D-0856CD372830}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9322CEF3-E682-498C-BB12-52667C1CED3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10864,7 +10864,7 @@
         <xdr:cNvPr id="154" name="文字方塊 153">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6AFEDB2-F994-4E9C-9709-6FFDFAA921CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{671A7377-CBCF-41A8-8920-D79402B15BB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10962,7 +10962,7 @@
         <xdr:cNvPr id="155" name="文字方塊 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4544A9D-D5AC-4712-815F-B44C02BE01CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFC0399C-4FD0-4B81-A050-F2D22F5F1CB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11060,7 +11060,7 @@
         <xdr:cNvPr id="156" name="文字方塊 155">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0017684-908E-472F-BCD6-56D8AAB074F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D7536B-2263-4268-9BD2-931890A18344}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11158,7 +11158,7 @@
         <xdr:cNvPr id="157" name="直線接點 156">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0DFF6A5-7F1B-4B78-8E32-DD2699250DB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B9166E8-FFDC-4724-A88A-705DC47E0562}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11213,7 +11213,7 @@
         <xdr:cNvPr id="158" name="直線接點 157">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0238979-D542-4E4B-B1F4-37516C4868D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C495CA38-05D2-4E34-8F2A-45168C4DFD5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11268,7 +11268,7 @@
         <xdr:cNvPr id="159" name="直線接點 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80C59882-53DE-4372-A17B-640ADF01969A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17D2BBFB-55A7-4D71-805C-BD8767636D0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11323,7 +11323,7 @@
         <xdr:cNvPr id="160" name="文字方塊 159">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10621956-A346-4CFF-9FD8-1F5846D1290A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD6C91AA-95B3-4867-8EDB-836BD92DF6F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11421,7 +11421,7 @@
         <xdr:cNvPr id="161" name="文字方塊 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ED810E8-683C-4927-8077-5FA2C4EF52EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0F6BD0F-4ABD-4A6B-A83D-F3B7C3EC062B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11519,7 +11519,7 @@
         <xdr:cNvPr id="162" name="文字方塊 161">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C5F79E-9715-4D4C-B849-1955844B9076}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADDFDD05-8941-441E-9E83-F6BFC1C3B90F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11617,7 +11617,7 @@
         <xdr:cNvPr id="163" name="直線接點 162">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78FB2973-7F07-4595-83EF-11CF3AC1983D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F86D7DC1-C39F-416B-A5C7-5FA99CCF16F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11672,7 +11672,7 @@
         <xdr:cNvPr id="164" name="直線接點 163">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35D0F51B-5B67-45D3-B841-D103BFF50419}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE2F6933-8892-4393-AA19-F5067BEEA839}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11727,7 +11727,7 @@
         <xdr:cNvPr id="165" name="直線接點 164">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E51BE85-34DB-4E7B-8CA2-152C76BA5CB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{015F36FB-9593-424C-B379-E0D77C2D6E44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11782,7 +11782,7 @@
         <xdr:cNvPr id="166" name="文字方塊 165">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C8F504-7F84-43D0-BC22-8B8F47803563}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167D0B47-63FA-4D29-803E-9130D4429953}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11880,7 +11880,7 @@
         <xdr:cNvPr id="167" name="文字方塊 166">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67524F7-8EC5-4577-8E68-69A237BCE467}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C1A1F8-15A7-4989-9EC2-7D83D40A3A91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11978,7 +11978,7 @@
         <xdr:cNvPr id="168" name="文字方塊 167">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91CCF1F-CAA2-45FB-B9E9-AE3B0E056E39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4217B1B-2ABD-4D58-9592-5DEB3DB432EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12076,7 +12076,7 @@
         <xdr:cNvPr id="169" name="直線接點 168">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD97F968-39D5-4049-A855-C30967E34DCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F6DD10-1631-4ADC-B4D9-E8D686DB3C56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12131,7 +12131,7 @@
         <xdr:cNvPr id="170" name="直線接點 169">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9DC625-EA06-4A51-8214-11C0E6E0EB1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CD25DDD-F116-4A8B-9DE0-ADB21F74BEFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12186,7 +12186,7 @@
         <xdr:cNvPr id="171" name="文字方塊 170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECAD7D5-2CCA-403B-A0F0-1B01C5935B8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E62FA8D-7BD4-4958-81D3-D10A399AC6C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12284,7 +12284,7 @@
         <xdr:cNvPr id="172" name="文字方塊 171">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{447F5540-321E-43CE-A467-C273F3BA1E40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECD8D87-CCCB-44FC-9D50-F21A3ADF95BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12382,7 +12382,7 @@
         <xdr:cNvPr id="173" name="直線接點 172">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D154F9CF-DBBC-44DD-B62B-F3E847EA7663}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3646990A-9D9A-4E21-9D3E-41A60DE7E4AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12437,7 +12437,7 @@
         <xdr:cNvPr id="174" name="直線接點 173">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE50692-128F-42D4-8EFF-E5109322533E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC047CB7-74F8-4F2E-B62D-8BEE2BF27F28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12492,7 +12492,7 @@
         <xdr:cNvPr id="175" name="直線接點 174">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE41D5E-3622-483A-B63B-046AEB20F621}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E74F28-3112-455D-B7F7-F8856CA2677E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12547,7 +12547,7 @@
         <xdr:cNvPr id="176" name="直線接點 175">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1769632-A050-4B67-8A84-D43EBB8F7A64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBAF3062-39B9-44A3-A761-6A4BAB7DC3D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12602,7 +12602,7 @@
         <xdr:cNvPr id="177" name="直線接點 176">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6A74A8-2D12-4833-A977-D746EC955587}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5AD5E53-16F3-440A-A4F8-00D6CD994DA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12657,7 +12657,7 @@
         <xdr:cNvPr id="178" name="直線接點 177">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CE6715-9910-4B3A-B1A3-E335F2EE7D5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3E4B530-CC6D-4610-B561-C66ADD27DF2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12712,7 +12712,7 @@
         <xdr:cNvPr id="179" name="弧形 178">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74446F8F-CE06-4D71-BDFB-E4389BD47961}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4503802D-D3A2-45C3-A7D8-8C5CF111A77A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12778,7 +12778,7 @@
         <xdr:cNvPr id="180" name="弧形 179">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{232145BF-30F5-414D-833F-0332F38707A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E22CD9-379B-4F1C-AE31-0AB0B191721E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12844,7 +12844,7 @@
         <xdr:cNvPr id="181" name="弧形 180">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EF34C37-0BB1-4F7A-9808-BABD9E956CFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BA355CE-AF47-4B47-BB81-30F65B9020E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12910,7 +12910,7 @@
         <xdr:cNvPr id="182" name="弧形 181">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC03543F-3343-470E-AF0C-72BDAC0EF3CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBFA92A6-33A7-4842-ADD3-2F59DC36CA32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12976,7 +12976,7 @@
         <xdr:cNvPr id="183" name="弧形 182">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A29085E7-1035-4C61-8179-C2AF1BAE5445}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F5A9EF1-3E91-4B36-A914-5A5BD3822C63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13042,7 +13042,7 @@
         <xdr:cNvPr id="184" name="文字方塊 183">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE7D769-F460-469F-9210-E7D81C81DE74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25FD8E7E-4964-443B-B9F4-733F8FCF15DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13140,7 +13140,7 @@
         <xdr:cNvPr id="185" name="文字方塊 184">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC95A9B-E730-487B-90B3-EE7DE3576259}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C579AE31-8C17-4EBD-8273-809FF8BAF7BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13238,7 +13238,7 @@
         <xdr:cNvPr id="186" name="文字方塊 185">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB470C8-5858-42DC-AA3E-5CD97F2E196B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F05671E0-E1DC-4E2E-96BB-E0B77271570C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13336,7 +13336,7 @@
         <xdr:cNvPr id="187" name="文字方塊 186">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A44020B-BE8F-4AE7-BDFF-4A406FFED876}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8CCDEF-A905-478B-9C99-5E0F91F0C0A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13434,7 +13434,7 @@
         <xdr:cNvPr id="188" name="文字方塊 187">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{163E0C82-8C96-43A3-9735-24A28E445B14}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2030C52-A192-42FF-9288-2F83E6BB41DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13532,7 +13532,7 @@
         <xdr:cNvPr id="189" name="直線接點 188">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD43D593-608C-489C-A2AE-98BB256F2F22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F23962-0100-47B8-A8F6-807258CD6092}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13587,7 +13587,7 @@
         <xdr:cNvPr id="190" name="直線接點 189">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45270E1B-E280-4668-B019-76F7F7E7744C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944A7166-B518-4392-893A-78BCBAFEAE17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13642,7 +13642,7 @@
         <xdr:cNvPr id="191" name="直線接點 190">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A382B0-0F70-4515-807F-343194F7749D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{699BBD7D-DFB0-497D-B962-D8D933552C5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13697,7 +13697,7 @@
         <xdr:cNvPr id="192" name="直線接點 191">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D423D81D-6BE2-4EA4-98BA-6817297BA5B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA38CF63-822E-43A4-8D25-CD673FA0D6AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13752,7 +13752,7 @@
         <xdr:cNvPr id="193" name="直線接點 192">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{363C2F2C-BEB8-4A7F-8DAF-8BD5404E8F16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{614760C9-F7FB-41CC-837E-D09AB48E82BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13807,7 +13807,7 @@
         <xdr:cNvPr id="194" name="弧形 193">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE9629CA-56C8-414B-B42D-F50BCFFC69CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A64403-1882-434A-B1E6-DA7FDF62B6CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13873,7 +13873,7 @@
         <xdr:cNvPr id="195" name="弧形 194">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478AA40A-6781-40F5-ADAF-1D7A882FAE22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E51F5971-3D8B-4615-8567-F21154082300}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13939,7 +13939,7 @@
         <xdr:cNvPr id="196" name="弧形 195">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66F964A3-FA61-46D9-9CB8-BDD219D8DCFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A255FF05-3F1A-40AF-BC05-7B4FE27E89AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14005,7 +14005,7 @@
         <xdr:cNvPr id="197" name="弧形 196">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5A955D-A786-4E4E-AE5D-7DBC4D23F454}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A281E5D-B285-48DE-81A8-AA24EE513727}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14071,7 +14071,7 @@
         <xdr:cNvPr id="198" name="文字方塊 197">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE1A900-734A-4C29-9271-551F972A7042}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5804EC7F-056D-4CD9-B42E-3190ACA382C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14169,7 +14169,7 @@
         <xdr:cNvPr id="199" name="文字方塊 198">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2BFD789-6E65-4144-AE6E-428DEFD6CC21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC2721D1-5614-4646-B7F3-95E67186594D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14267,7 +14267,7 @@
         <xdr:cNvPr id="200" name="文字方塊 199">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{723901BE-9388-4472-9AB0-A571FAE22C96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B2E5E2D-6EF4-47AE-80F9-E804A5ABC724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14365,7 +14365,7 @@
         <xdr:cNvPr id="201" name="文字方塊 200">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6D5B1C-4C11-42D5-AA88-F61919B18116}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C392F5-7B87-466F-92A1-B7E78B84B253}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14463,7 +14463,7 @@
         <xdr:cNvPr id="202" name="文字方塊 201">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C71E6DD-0EBD-41A4-BDFE-A83366C61DCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{201C3D79-3E1B-480F-B67C-F845A7C93F40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14561,7 +14561,7 @@
         <xdr:cNvPr id="203" name="直線接點 202">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D740DA3-04AA-4F9D-A2AF-621BC0BBAFF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D60F90-B019-4917-A4AA-B1187A2C5578}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14616,7 +14616,7 @@
         <xdr:cNvPr id="204" name="直線接點 203">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E9F64A2-E42D-4496-A14C-B3F5DDE72290}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9B0218A-EEF4-4D7A-8333-62F34D42D9A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14671,7 +14671,7 @@
         <xdr:cNvPr id="205" name="直線接點 204">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80E3549-E2E0-458A-A99E-4715018142FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B291E5-9776-4161-B6BE-AB724620D98E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14726,7 +14726,7 @@
         <xdr:cNvPr id="206" name="弧形 205">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{648EE8DD-7909-45BB-9EB9-ABE72F5AE627}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD9DEB21-C35D-43C5-95A6-35A5A909DD5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14792,7 +14792,7 @@
         <xdr:cNvPr id="207" name="弧形 206">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D715499-5DA9-4169-B3BB-FB86B88B0F62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CFFCADC-DB16-4061-8DD8-E8191FB4851B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14858,7 +14858,7 @@
         <xdr:cNvPr id="208" name="文字方塊 207">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF0C95F-DB06-43FD-A88A-D2CB32118CF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB55F0A-0F6E-4173-B25F-ADD3B7F1F13C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14956,7 +14956,7 @@
         <xdr:cNvPr id="209" name="文字方塊 208">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD83E1B2-043F-4E75-A83A-553105ACE7C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74EAB271-950D-4B7E-9D38-CDA6A4E53C10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15054,7 +15054,7 @@
         <xdr:cNvPr id="210" name="文字方塊 209">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77BBD1B4-ACF8-4964-B44D-A34E53D1F77F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C64EBCB-F57B-47E4-93BF-BF9F6B1A5E31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15152,7 +15152,7 @@
         <xdr:cNvPr id="211" name="文字方塊 210">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ACB35DA-8CD2-400C-A53B-77DFD7BFF895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69632690-5023-498F-9124-1881B6C1E5C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15250,7 +15250,7 @@
         <xdr:cNvPr id="212" name="文字方塊 211">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D3CED9-5F78-4DBE-8726-D751FE6B80E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EF72964-58B2-4523-9A54-4657234AE158}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15348,7 +15348,7 @@
         <xdr:cNvPr id="213" name="直線接點 212">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6A8C74-EDBB-4493-9288-5DDF552B781C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED65217A-C760-47BD-8131-29B5C4B9BF2F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15403,7 +15403,7 @@
         <xdr:cNvPr id="214" name="直線接點 213">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6EB7AC-6412-4B0A-B4AD-3FA68D4F18CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B955028-196F-4420-99B5-AA5610A897A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15458,7 +15458,7 @@
         <xdr:cNvPr id="215" name="直線接點 214">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56BB5770-4E51-4296-BA19-0D575668BED5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A33D19E-F049-460D-A610-E75653A05D1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15513,7 +15513,7 @@
         <xdr:cNvPr id="216" name="直線接點 215">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D945000A-7E59-4B5D-B809-6C386E280A2F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219EDF0D-68F9-4034-880D-A4902CA7A3DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15568,7 +15568,7 @@
         <xdr:cNvPr id="217" name="直線接點 216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CE8A24E-ED20-4351-A589-F79F2A04BDEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E11B8D3-A4E9-45A1-821B-8E934CC1F6A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15623,7 +15623,7 @@
         <xdr:cNvPr id="218" name="直線接點 217">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB535252-2080-4982-A79A-8257EA671129}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D21CB4-C22E-4039-9707-A4E18C05D89E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15678,7 +15678,7 @@
         <xdr:cNvPr id="219" name="弧形 218">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DCE55EE-B920-4FA1-9314-91292766FDAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A77FBA2E-9BB7-436F-9B6D-F13D0AB95A05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15744,7 +15744,7 @@
         <xdr:cNvPr id="220" name="弧形 219">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77AF033D-299B-4E88-8682-3E6A985C2EFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E6B707-DB75-4A00-A906-EB630ED94881}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15810,7 +15810,7 @@
         <xdr:cNvPr id="221" name="弧形 220">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33515AC-9B9F-43DC-AF87-3CE48533593A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B04492A-8571-424C-A5E9-FA3D05F75D94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15876,7 +15876,7 @@
         <xdr:cNvPr id="222" name="弧形 221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA699927-A3BD-4808-8D7C-247B4178FC9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5944D3BF-0426-43C9-AB83-FF85E1A80C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15942,7 +15942,7 @@
         <xdr:cNvPr id="223" name="弧形 222">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F978C499-7C29-42E7-830A-1E6B0DE7B341}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81221C9D-906D-4865-A971-74E603F859E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16008,7 +16008,7 @@
         <xdr:cNvPr id="224" name="文字方塊 223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3393F7E8-5843-41DB-9685-C73D2761795D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9648339C-6C1E-4EC4-AA5F-3A2E6CD4C44C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16106,7 +16106,7 @@
         <xdr:cNvPr id="225" name="文字方塊 224">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CCFAAF5-F97A-4DF7-8701-FF6AC2FADB31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1E5BC6-C839-4C72-A89D-E67329B74384}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16204,7 +16204,7 @@
         <xdr:cNvPr id="226" name="文字方塊 225">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C51C130-BD99-47AB-869B-8988D21898ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B28A991-5C01-48F0-B9D6-3799484BE40A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16302,7 +16302,7 @@
         <xdr:cNvPr id="227" name="文字方塊 226">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{347BBCBB-5DB9-4167-971F-DBFAF0C3DF26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72734FA6-9C6A-48D8-B27D-6AA459DF4F5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16400,7 +16400,7 @@
         <xdr:cNvPr id="228" name="文字方塊 227">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FDFBC9-E647-4706-B778-292B65EA3411}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59473C21-D601-4257-B444-A6B1EB12CDD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16498,7 +16498,7 @@
         <xdr:cNvPr id="229" name="直線接點 228">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D99A146D-68F3-45EC-8D9F-E2CDCC94494D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFB5AC96-4C08-41A3-B16A-8DE57336CF5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16553,7 +16553,7 @@
         <xdr:cNvPr id="230" name="直線接點 229">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C61B70-4160-4AD3-ACE7-3DC10D9B7023}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55277959-7C09-4858-A11D-4A3A606B3702}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16608,7 +16608,7 @@
         <xdr:cNvPr id="231" name="直線接點 230">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBF1388C-2FE3-445A-BE09-55D82D1B1763}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2278991B-3EFD-4ACC-8C6B-575A4B95296F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16663,7 +16663,7 @@
         <xdr:cNvPr id="232" name="直線接點 231">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8C276A-77BA-467A-9CA2-066E5BB546C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A54AB3D-C7B4-431A-90CD-521A6B5CC3BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16718,7 +16718,7 @@
         <xdr:cNvPr id="233" name="直線接點 232">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30408127-5165-484F-BA8C-E3C42927D6A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2478B40E-721B-4F6B-90C9-B86009E357D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16773,7 +16773,7 @@
         <xdr:cNvPr id="234" name="直線接點 233">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806BFFA7-2723-4732-8393-195E53D0D959}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94577201-65A4-454E-ADDD-F080AD897D65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16828,7 +16828,7 @@
         <xdr:cNvPr id="235" name="弧形 234">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BD5F096-EBE3-413D-A5C1-B16F598A439A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE1AE82A-3780-44D8-B5BD-1A75677777C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16894,7 +16894,7 @@
         <xdr:cNvPr id="236" name="弧形 235">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F22A9F7-87D3-4B22-9679-D9605A873496}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C44742B6-41F4-46A7-9E69-DB86403DEEBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16960,7 +16960,7 @@
         <xdr:cNvPr id="237" name="弧形 236">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{229A3967-854F-4C7B-A2E5-747ADC638ADF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9487EF30-0E0D-44D5-ABF7-326285190598}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17026,7 +17026,7 @@
         <xdr:cNvPr id="238" name="弧形 237">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A94185-E043-4B24-AA24-686A1CA7930D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3DC70E5-6E25-4AC7-9A00-5371A39489E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17092,7 +17092,7 @@
         <xdr:cNvPr id="239" name="弧形 238">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BD7FAE7-45AF-468C-B6BB-341F8C639D32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99ABD31F-352C-49F2-810D-C500796055CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17158,7 +17158,7 @@
         <xdr:cNvPr id="240" name="文字方塊 239">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA363144-6D1B-400B-8F07-B7C3276A9801}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7073B54B-713B-454F-A24B-C1B2E4B15A02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17256,7 +17256,7 @@
         <xdr:cNvPr id="241" name="文字方塊 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21354654-6A20-4967-AE17-B20AA9D64DE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C88F72C-1CE3-4072-AAD9-11A688A0A27A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17354,7 +17354,7 @@
         <xdr:cNvPr id="242" name="文字方塊 241">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F13CD9D-BE99-4F85-977E-C84EA3E0A6F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD22F469-DD26-4659-9806-4151DDDDF6A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17452,7 +17452,7 @@
         <xdr:cNvPr id="243" name="文字方塊 242">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E21D1F8-D254-489F-A94F-B1F1F1F9F7C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36E58028-DD61-4E17-9611-4416040F1C53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17550,7 +17550,7 @@
         <xdr:cNvPr id="244" name="文字方塊 243">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAD96C13-B0EF-4864-BAFD-399B2AEFC28B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47F6D391-3DAC-47B7-AF87-A61DB91BD1BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17648,7 +17648,7 @@
         <xdr:cNvPr id="245" name="直線接點 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A81F9CD3-A93C-4136-A1EE-53389B03D416}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A58E4430-B836-4183-B0E6-2F6717DDB21A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17703,7 +17703,7 @@
         <xdr:cNvPr id="246" name="直線接點 245">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD9E9B4-CD97-49A3-BCD6-988EF590F3E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{957E0A00-52E3-47A4-A3DA-1684594AC383}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17758,7 +17758,7 @@
         <xdr:cNvPr id="247" name="直線接點 246">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F154301-758E-4F35-A02E-57BF0827BE91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CBA8E03-4F1A-4484-9911-B0A725B160E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17813,7 +17813,7 @@
         <xdr:cNvPr id="248" name="直線接點 247">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10CE7442-6AB1-4748-9F5D-A6D9F080D0C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF353ED7-DB57-42DE-981D-02FC4B81DEC7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17868,7 +17868,7 @@
         <xdr:cNvPr id="249" name="弧形 248">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B68F3A0-2176-4B92-B989-859680F9F06F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD6D9EE-EE18-4C0C-AC25-4A80893AB70C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17934,7 +17934,7 @@
         <xdr:cNvPr id="250" name="弧形 249">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B33540-2514-4532-93CD-C51EAD45F2E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A35C1664-3687-4F44-93F4-F91A4DA87F59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18000,7 +18000,7 @@
         <xdr:cNvPr id="251" name="文字方塊 250">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F521D6CB-7003-41A4-987A-40E6085D61F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B815C4EF-EBA9-46E0-9F9B-56DCE2FAD9E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18098,7 +18098,7 @@
         <xdr:cNvPr id="252" name="文字方塊 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ADD23C5-2A8F-4E27-830F-01CE767CE6C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C0C6D54-46CF-40E2-A208-BF3CDF0407F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18196,7 +18196,7 @@
         <xdr:cNvPr id="253" name="文字方塊 252">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5353CAE4-459A-45E1-B00E-8EF66A705F42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DA45B8F-8250-4B98-A90E-9D3C501FAE0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18294,7 +18294,7 @@
         <xdr:cNvPr id="254" name="文字方塊 253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{775B2E3D-1066-422F-B3C5-A27725C7ED64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A36A24-0C59-47E7-B4E7-CEEE12E17562}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18392,7 +18392,7 @@
         <xdr:cNvPr id="255" name="直線接點 254">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6AC04A6-8C72-4345-A9FA-A4FF8B90337D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF63BD71-2601-4896-97F6-FB09BF7E3885}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18447,7 +18447,7 @@
         <xdr:cNvPr id="256" name="直線接點 255">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D081292F-2566-45B3-8E81-A3B8857B53FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A21594-C479-41DC-9B14-8EF3978B2BD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18502,7 +18502,7 @@
         <xdr:cNvPr id="257" name="直線接點 256">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F4BC4F-E8D1-4DF7-897B-7A45A91F49D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A48E3F-2FD1-41E5-BE3B-703BAC583B5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18557,7 +18557,7 @@
         <xdr:cNvPr id="258" name="直線接點 257">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E04A0B1-2220-4FF5-86D9-F02DFF95E458}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF89D2B-109C-4591-AE03-057CD264DB8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18612,7 +18612,7 @@
         <xdr:cNvPr id="259" name="直線接點 258">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1B6B9C-2D92-47D9-AB65-E2E9E9BB52C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6723D59A-4AE3-4888-8131-1B367E324610}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18667,7 +18667,7 @@
         <xdr:cNvPr id="260" name="弧形 259">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17937706-E4BF-47A1-AE9A-2043A351CA07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7329F7B1-B494-41F3-BE2D-E8AA67EC510B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18733,7 +18733,7 @@
         <xdr:cNvPr id="261" name="弧形 260">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85438765-3F4D-4509-A78D-39169448B6B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CFA14A6-FBEB-4844-97B6-E0A13378F45D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18799,7 +18799,7 @@
         <xdr:cNvPr id="262" name="文字方塊 261">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6471D04-40C8-4908-AE6D-DD802CCC7948}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2636A22-684D-41B9-8B31-253AB5A56565}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18897,7 +18897,7 @@
         <xdr:cNvPr id="263" name="文字方塊 262">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F95F0EC-FFCA-49AD-BDE7-98B01EF77B5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{874A7564-7F03-4071-AA30-9D6326FE136D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18995,7 +18995,7 @@
         <xdr:cNvPr id="264" name="文字方塊 263">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5841C01-B563-413D-AEAC-470DF743D1A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DA21ED-E3AA-4146-ABF7-7C67C3B94CCE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19093,7 +19093,7 @@
         <xdr:cNvPr id="265" name="文字方塊 264">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC7EC84-E44D-4294-B86B-733A391B40E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD75A32-F2CF-4A5D-AF2A-39934C314718}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19191,7 +19191,7 @@
         <xdr:cNvPr id="266" name="文字方塊 265">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DFCD38-EC25-4CA0-A755-4CD8FF61CEAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCC5EAD-0C58-4258-9177-89BA0BA12587}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19289,7 +19289,7 @@
         <xdr:cNvPr id="267" name="直線接點 266">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87ACF708-11B5-4DE3-BD64-DC96A88E4985}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{780EDED5-96A4-46CB-B5F6-D8DFBA3665FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19344,7 +19344,7 @@
         <xdr:cNvPr id="268" name="直線接點 267">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D764C499-A13B-4776-86A0-A69BD2184C0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028F3BC4-1ED0-4EC4-81F5-5A1D93869469}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19399,7 +19399,7 @@
         <xdr:cNvPr id="269" name="直線接點 268">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81DFF42-DE29-492A-88EE-6A310D1F08AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{414D9A80-A8E1-4888-BB46-CAFC44C0E661}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19454,7 +19454,7 @@
         <xdr:cNvPr id="270" name="直線接點 269">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20B4E25-8A6C-4575-8B1A-4F5F706C92F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7DA5179-C0ED-4A92-B781-27EEF9774606}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19509,7 +19509,7 @@
         <xdr:cNvPr id="271" name="直線接點 270">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C80EE23-CB7E-43F9-ACB7-A628C9CAD053}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFBFCD4-078F-4E1C-A705-21C275553943}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19564,7 +19564,7 @@
         <xdr:cNvPr id="272" name="弧形 271">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90A2C1C-B318-4CB6-BB02-5E0D1D1F5215}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92ECF357-339B-4519-AC1D-206263CE8666}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19630,7 +19630,7 @@
         <xdr:cNvPr id="273" name="弧形 272">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4AB035-FF16-4446-AE66-663D026F8F05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7CAAA33-7B26-4C8A-9C6C-9FFCC7E887B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19696,7 +19696,7 @@
         <xdr:cNvPr id="274" name="文字方塊 273">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F4E6A25-4C8E-4774-8A0B-3D91E336DC9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D50ADF2-7FCC-4862-842A-BB8443824B28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19794,7 +19794,7 @@
         <xdr:cNvPr id="275" name="文字方塊 274">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2482E13-046C-49CF-8580-DEF319681A6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A3A84C2-E51F-4162-887F-CE85DB2942BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19892,7 +19892,7 @@
         <xdr:cNvPr id="276" name="文字方塊 275">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E03A409D-99C6-4A20-B9B2-2A997E94EF4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B8A4C3-7C05-46EB-B1DF-2D8CAC78E891}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19990,7 +19990,7 @@
         <xdr:cNvPr id="277" name="文字方塊 276">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A869AB18-64FA-40A7-B826-4A5CC42341B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDABEA99-6F9D-4D27-B842-FC0AA581CB70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20088,7 +20088,7 @@
         <xdr:cNvPr id="278" name="文字方塊 277">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20968515-D604-4D77-982B-666C493BEAA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8912CBF-21BB-4442-8DF4-E43EFB8CA8A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20186,7 +20186,7 @@
         <xdr:cNvPr id="279" name="直線接點 278">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{162E2E36-992E-4840-AF95-C82B031E6D1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6A1F44-6C97-4D11-85E4-D413B1F9BC20}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20241,7 +20241,7 @@
         <xdr:cNvPr id="280" name="直線接點 279">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8311574-6F9C-499F-B525-5A39D89EEECC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01020813-F977-4241-9FFB-7B1FC1A9C8E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20296,7 +20296,7 @@
         <xdr:cNvPr id="281" name="直線接點 280">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF398AA2-300F-4978-B9D4-A8C27DF0187A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F1848E-97DA-447F-A3D9-CD10F33401ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20351,7 +20351,7 @@
         <xdr:cNvPr id="282" name="弧形 281">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44FC4877-89BF-429C-897F-6A2A5F7DE853}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19511700-CBE6-4D3D-9FAD-BE75FA7214A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20417,7 +20417,7 @@
         <xdr:cNvPr id="283" name="弧形 282">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20BC63C-8DDA-4270-A6E0-B515DFE774E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC91AEC2-DEAF-4EBD-906F-7C534EB99B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20483,7 +20483,7 @@
         <xdr:cNvPr id="284" name="文字方塊 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6A4AD3A-F240-4748-A494-84BEFF6FA913}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2102EAF-88D3-40CC-B2B6-9C7CE381751E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20581,7 +20581,7 @@
         <xdr:cNvPr id="285" name="文字方塊 284">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6834BE6A-4BE8-4E05-B1B5-C8ADA45F9E0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB17AFC5-F732-43A6-B5B9-8297E8EFE79C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20679,7 +20679,7 @@
         <xdr:cNvPr id="286" name="文字方塊 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A3635C-DA59-4EE9-9473-A72BB4C07A41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB656D8-54C1-4232-91C9-73115F80CAEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20777,7 +20777,7 @@
         <xdr:cNvPr id="287" name="文字方塊 286">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5C10184-58DF-41F3-A94E-8809A4C490D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8918FBD0-8FCA-4539-9C78-1E9953ED5279}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20875,7 +20875,7 @@
         <xdr:cNvPr id="288" name="文字方塊 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C83A606-A3F7-4A1A-A55F-41BA007ABE93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B22E0E0-3F39-4781-9528-9ACA083744AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20973,7 +20973,7 @@
         <xdr:cNvPr id="289" name="直線接點 288">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3DF7A1D-DC35-469E-B786-07F8BA04FBBC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16547C5D-8564-4EA1-98E8-9A52ACC82A41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21028,7 +21028,7 @@
         <xdr:cNvPr id="290" name="直線接點 289">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21A4979-6129-4C7E-9450-F0694418B8FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2BFA9A3-5E08-4A55-B31B-08D784C1221E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21083,7 +21083,7 @@
         <xdr:cNvPr id="291" name="直線接點 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17ADC174-7649-4DAA-BA47-7868BB4A62C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB95C868-0D55-40A0-B4F9-991A9D4C9F2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21138,7 +21138,7 @@
         <xdr:cNvPr id="292" name="直線接點 291">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A48EE96A-0A52-4FAC-A16B-E402452F918D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0760DFFA-E48B-46D8-B233-67BA1FF221C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21193,7 +21193,7 @@
         <xdr:cNvPr id="293" name="弧形 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA49C66-E12C-44CE-A00B-5997F530360D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A9BDD39-5309-40DE-A753-AEF0A7F552E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21259,7 +21259,7 @@
         <xdr:cNvPr id="294" name="弧形 293">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61C1ADD4-73A3-4E3E-A6E7-8F1893DF6BCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35C73ED-8360-4D4E-A5E1-BFA837B3C078}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21325,7 +21325,7 @@
         <xdr:cNvPr id="295" name="弧形 294">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B96731B-5B53-4F6B-A7CC-0E8E81329DA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6738A01E-D435-4AD7-9B2C-6749FEDEBEEA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21391,7 +21391,7 @@
         <xdr:cNvPr id="296" name="文字方塊 295">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA3C203-2510-473E-A65B-0654DD790432}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0715E044-643B-496B-97C8-CE17D1FFF1B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21489,7 +21489,7 @@
         <xdr:cNvPr id="297" name="文字方塊 296">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4DDC9F-1AA7-4265-B229-AF86A6C56EA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94CDAF65-23FF-4F4D-A290-A7FA63893CC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21587,7 +21587,7 @@
         <xdr:cNvPr id="298" name="文字方塊 297">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33B5BF7-A7F8-411D-9E73-2D78A1BEBFC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECE57A2B-AAEF-4138-80A8-BD4280E5C932}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21685,7 +21685,7 @@
         <xdr:cNvPr id="299" name="文字方塊 298">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A94571-E3DE-40AD-8CFC-66180C7A64B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1800846-EFCC-475B-AB01-E538F921D102}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21783,7 +21783,7 @@
         <xdr:cNvPr id="300" name="直線接點 299">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B71015-1EE9-44AE-96AB-8EDDD166CB3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE007BC-3D36-4129-AF8C-F8EABD6A2097}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21838,7 +21838,7 @@
         <xdr:cNvPr id="301" name="直線接點 300">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD08DDB5-F023-4765-A944-AEB69E4715BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA5709B3-5453-4DFD-8C1B-0170EE1BD923}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21893,7 +21893,7 @@
         <xdr:cNvPr id="302" name="直線接點 301">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA408F62-2718-4902-A571-86D06DA68558}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C42DA1-516E-45E8-B06A-D961B76A14ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21948,7 +21948,7 @@
         <xdr:cNvPr id="303" name="弧形 302">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF8812D3-DA81-4B8A-BB55-020F72D76B0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DB90C6-692C-4B8B-8F22-3E5494A7F884}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22014,7 +22014,7 @@
         <xdr:cNvPr id="304" name="弧形 303">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5565240E-7D4D-44E9-B45F-0ED1480EC617}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D80B65D3-B69A-4FBE-8F06-A7EFCF8187CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22080,7 +22080,7 @@
         <xdr:cNvPr id="305" name="文字方塊 304">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4135DD9F-FC67-450B-95CC-94EB5ED4C1A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84AE4C65-FACA-4C04-B357-9345183C9DB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22178,7 +22178,7 @@
         <xdr:cNvPr id="306" name="文字方塊 305">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C27E5AE-159D-4CEF-9576-A2C877211DAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB216BD2-4067-466F-8487-B915CEC1F4B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22276,7 +22276,7 @@
         <xdr:cNvPr id="307" name="文字方塊 306">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EB898F8-D21D-4971-B733-A24A3BCC2ED2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5833CA2F-DA12-43BA-A5E3-58F8E55D1AD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22374,7 +22374,7 @@
         <xdr:cNvPr id="308" name="文字方塊 307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCE1C98A-C3E2-4A26-A34C-75B78B8625BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64F8F13-1196-451E-BEDD-322320C213A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22472,7 +22472,7 @@
         <xdr:cNvPr id="309" name="文字方塊 308">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83192218-B1AF-434A-BB86-00F25C23F931}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CC2213-CF5B-49B9-ACC7-BB6BB010ACCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22570,7 +22570,7 @@
         <xdr:cNvPr id="310" name="直線接點 309">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9EB51D8-32E5-4DA4-8465-A1802D1C923A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{138B0058-7FCB-499C-98DF-2C6BF83BF06B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22625,7 +22625,7 @@
         <xdr:cNvPr id="311" name="直線接點 310">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D965CD6F-2CBD-474A-A18C-12D80FE8F42F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6179FC8-1EDF-424E-B851-52407754230F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22680,7 +22680,7 @@
         <xdr:cNvPr id="312" name="直線接點 311">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7389F535-1C36-468E-A405-8C7787DF2D3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EAFC023-1F65-4625-AB3D-4D0C8448893B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22735,7 +22735,7 @@
         <xdr:cNvPr id="313" name="弧形 312">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1275C96-ECEF-44D2-BA34-441FE155F3B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A507D6F4-18E3-4050-93C5-76B21D05853F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22801,7 +22801,7 @@
         <xdr:cNvPr id="314" name="弧形 313">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94ADB125-E2F7-4DA6-91F6-5700A09689E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E521D3CC-2C91-4B96-9A94-E3E06DB760B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22867,7 +22867,7 @@
         <xdr:cNvPr id="315" name="文字方塊 314">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C0E95D-13A3-4BD3-9AF3-7C789CA59D2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A4C98E0-B320-4C92-B8E8-51F3F45FE0A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22965,7 +22965,7 @@
         <xdr:cNvPr id="316" name="文字方塊 315">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DB16001-9997-41E2-B29D-B0CF579F8271}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F9E99AA-E12F-4613-A894-54D20C747500}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23063,7 +23063,7 @@
         <xdr:cNvPr id="317" name="文字方塊 316">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48DAD29-45B5-47C1-B4A4-FA7B47559A5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFFF2C70-7D41-4316-B58F-7F9DB1C98093}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23161,7 +23161,7 @@
         <xdr:cNvPr id="318" name="文字方塊 317">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7FFB210-B781-4300-B511-27CA66889DCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A19CAB80-8B81-48A3-9695-D7961EE9BBD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23259,7 +23259,7 @@
         <xdr:cNvPr id="319" name="文字方塊 318">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BC17DB-C85A-43C6-B8B1-AD05B08C8CEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0203EE0A-FE23-42EB-9366-885F5EF7A36A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23357,7 +23357,7 @@
         <xdr:cNvPr id="320" name="直線接點 319">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77C8AEEE-D18C-49C5-8B76-D2505B152A4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA8B758-F758-455D-9E37-51F761A7A707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23412,7 +23412,7 @@
         <xdr:cNvPr id="321" name="直線接點 320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4611954A-6DEE-4114-AF05-A8B4696F6A2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4AA1327-6C97-4C32-8B21-DC05B626E5AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23467,7 +23467,7 @@
         <xdr:cNvPr id="322" name="直線接點 321">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A6C2F74-8772-491E-AF89-2C559DCAEB43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318F4A86-36A3-4FFC-ADD4-04B47875C37A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23522,7 +23522,7 @@
         <xdr:cNvPr id="323" name="弧形 322">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7035BBAD-0FAE-4141-B832-6FD8129E9B54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAFD93EA-880E-4CB8-8624-8B56E250E322}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23588,7 +23588,7 @@
         <xdr:cNvPr id="324" name="弧形 323">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6103FD71-3FD4-4B33-AA8A-171767EDE639}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871D4D7D-D463-4F67-8D26-64C7D42BDE05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23654,7 +23654,7 @@
         <xdr:cNvPr id="325" name="文字方塊 324">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB44A9A9-1DD5-4130-9A25-B16BDCDD976E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D960CD67-0CAA-45E3-82CD-EEFE545F6751}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23752,7 +23752,7 @@
         <xdr:cNvPr id="326" name="文字方塊 325">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10A8C3B-65DF-4702-BF2F-CA67FAE381BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A17E801-C3A1-455C-89F6-2416AFE70252}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23850,7 +23850,7 @@
         <xdr:cNvPr id="327" name="文字方塊 326">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D185A5B-DC11-42AB-93CC-2D61C028F361}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1C1189-864D-4C19-B23F-69595DE16122}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23948,7 +23948,7 @@
         <xdr:cNvPr id="328" name="文字方塊 327">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5257D03E-3C07-4A98-999D-2F07B312E748}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5065A6-C9CD-455B-81A8-391B26C6A154}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24046,7 +24046,7 @@
         <xdr:cNvPr id="329" name="文字方塊 328">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA5D96A-C546-486B-BC50-3A0D398987DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2ACE97-C658-4AB7-A3B8-9CC6FF070498}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24144,7 +24144,7 @@
         <xdr:cNvPr id="330" name="直線接點 329">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6FD163-0225-4C5B-90BE-BCA55799ABBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE3C48A0-5213-4724-8CDD-991D80FD8002}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24199,7 +24199,7 @@
         <xdr:cNvPr id="331" name="直線接點 330">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97641BA2-7DEC-42E0-9242-5D271834B56C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58DE0DBF-C5A0-40A2-A421-5ABA5DCB4DC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24254,7 +24254,7 @@
         <xdr:cNvPr id="332" name="直線接點 331">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A89CD191-878A-43F0-B9C4-D781EC25786E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5847A88D-F553-41A0-9405-2F7505EE70CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24309,7 +24309,7 @@
         <xdr:cNvPr id="333" name="弧形 332">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE28EA4C-FCDA-44E5-B62B-B2EE0B8E87EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929EE0E7-8FF1-4550-BEF3-B86593C13000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24375,7 +24375,7 @@
         <xdr:cNvPr id="334" name="弧形 333">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC71BB1-5D79-441A-85C1-1A5F10E74678}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9F86E44-E8F8-4C66-B94C-E52E8C1F4C70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24441,7 +24441,7 @@
         <xdr:cNvPr id="335" name="文字方塊 334">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0250B9D7-3966-4B6C-A59F-E3E95A6CB2CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2370812-A2E3-4223-9EAE-DDD26F7DF86E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24539,7 +24539,7 @@
         <xdr:cNvPr id="336" name="文字方塊 335">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33ADA871-0D7D-439F-8EA5-5C72BB8FD4C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E8FE6FB-741C-4A2C-8065-80839A5C6160}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24637,7 +24637,7 @@
         <xdr:cNvPr id="337" name="文字方塊 336">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{846604AD-5984-400F-8028-41BA3CF51B08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BF76851-B254-4647-B102-87103C0069E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24735,7 +24735,7 @@
         <xdr:cNvPr id="338" name="文字方塊 337">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D879011-E9CA-49E5-A465-87F0F119D3E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28DB4F85-40AF-4CD4-868E-DBE50180CB0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24833,7 +24833,7 @@
         <xdr:cNvPr id="339" name="文字方塊 338">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D26DE55-FBB4-47B3-810F-AB63294290C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124C5C40-B0CD-4AC2-8069-6EF0240309C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24931,7 +24931,7 @@
         <xdr:cNvPr id="340" name="直線接點 339">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{504E9391-9D3D-4775-8CA8-2F454DE6428D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C11D98-C499-4A60-8ADB-A6B8641E77F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24986,7 +24986,7 @@
         <xdr:cNvPr id="341" name="文字方塊 340">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B68EECF-D1B7-4D97-9C15-EFA8190526E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2FCBD63-F024-43C2-949C-D6967845206D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25084,7 +25084,7 @@
         <xdr:cNvPr id="342" name="直線接點 341">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45748ACD-4122-4F4E-A3B9-77906DD3B517}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEE30D4C-8E63-4BF1-9B6A-F7CDCBECAB53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25139,7 +25139,7 @@
         <xdr:cNvPr id="343" name="直線接點 342">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{520CF88C-F0CA-496E-A481-8827DD3BADB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B562113-0FD2-4000-8522-C2909B5320BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25194,7 +25194,7 @@
         <xdr:cNvPr id="344" name="直線接點 343">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2B659D-9851-4F68-A0DC-20F9E11448B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E6ED9F8-FA99-45A0-9D52-9379105D078D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25249,7 +25249,7 @@
         <xdr:cNvPr id="345" name="直線接點 344">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D9B21C-F029-43B1-8453-85C9294CBD9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{376CB1A5-A803-4445-ACDA-E8D430F0A086}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25304,7 +25304,7 @@
         <xdr:cNvPr id="346" name="直線接點 345">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27E51093-1B22-4AD7-B1BD-003B38575BB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A1A5C6-D83B-4C51-8CBD-C60D9B3AA15E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25359,7 +25359,7 @@
         <xdr:cNvPr id="347" name="弧形 346">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A63E3E57-D8D3-4B85-8AB8-ABD507D54214}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75BB3FDD-251F-4C51-8791-D61FD9E28C6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25425,7 +25425,7 @@
         <xdr:cNvPr id="348" name="弧形 347">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E05C253A-AA20-41A7-A44C-A044ED89C5F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D866735-18B6-473E-A50D-B9A0A4B75E1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25491,7 +25491,7 @@
         <xdr:cNvPr id="349" name="弧形 348">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30C84DED-ED50-4E95-9D5B-EAA626D9CA98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C7C2CCC-207A-4DEE-AC3F-0C16D112CA2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25557,7 +25557,7 @@
         <xdr:cNvPr id="350" name="弧形 349">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4425666-48EC-4A7C-A140-CB47231AC7FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D33DDB-BCD2-4E45-B34D-7D2F62FACC2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25623,7 +25623,7 @@
         <xdr:cNvPr id="351" name="文字方塊 350">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBCA439C-4523-458D-B186-C07394044837}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310DCD27-5D28-4CA9-955C-14805469768F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25721,7 +25721,7 @@
         <xdr:cNvPr id="352" name="文字方塊 351">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A407D804-4490-4F65-AEC7-41C2FE31AEFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BA94DD-5103-400C-8B5B-CD8937CBC6CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25819,7 +25819,7 @@
         <xdr:cNvPr id="353" name="文字方塊 352">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F08606C6-6220-4336-89A9-6AEE0D93E6CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77D6AA95-515C-44BA-B7C8-56780C70AD60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25917,7 +25917,7 @@
         <xdr:cNvPr id="354" name="文字方塊 353">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29FEFAC0-4516-47D8-ACBF-471880E7AAEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8BF790E-815F-4EEE-950D-469C0F3EFEF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26015,7 +26015,7 @@
         <xdr:cNvPr id="355" name="文字方塊 354">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FF9B11-9F94-420B-AA6E-F634620EC9DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46CE2C02-FFB0-428A-80CD-083ADB891373}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26113,7 +26113,7 @@
         <xdr:cNvPr id="356" name="文字方塊 355">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B0CAC50-9579-4548-9B31-C56C565A9D95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DECC1A4-4567-4DFD-A182-25A3A25ECE33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26211,7 +26211,7 @@
         <xdr:cNvPr id="357" name="直線接點 356">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABB265CB-E14D-4D4D-8B23-409E3A126690}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A56D1A6-C532-44E3-A641-0E7E28EA771D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26266,7 +26266,7 @@
         <xdr:cNvPr id="358" name="直線接點 357">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA3152F-D75D-4C20-A23F-DDE012C9D9F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AAC12DE-D25D-4551-995F-699CEC03AB98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26321,7 +26321,7 @@
         <xdr:cNvPr id="359" name="直線接點 358">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6909C6F-9D16-4A7D-955C-393892EAA12D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEE7FD1-65AD-4053-B6DF-B9A70232551D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26376,7 +26376,7 @@
         <xdr:cNvPr id="360" name="直線接點 359">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A14F80-72E6-411A-93DC-102757C119E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F36B36-9383-49B7-89FD-2AEDC45DF16F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26431,7 +26431,7 @@
         <xdr:cNvPr id="361" name="弧形 360">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3B786C-A122-499C-997B-58319BC09422}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98E7F79-4EEF-43AB-8D08-BF54F1BEDED3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26497,7 +26497,7 @@
         <xdr:cNvPr id="362" name="弧形 361">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B41D95-EC88-49B0-9BAD-696740DBC436}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A089360-386A-4C45-8329-11678818A5F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26563,7 +26563,7 @@
         <xdr:cNvPr id="363" name="弧形 362">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F85A594-2745-425F-9298-C6D9DB1751E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88106584-99F9-4F3C-BF87-449DA46DF0FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26629,7 +26629,7 @@
         <xdr:cNvPr id="364" name="文字方塊 363">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CFDCD7D-8394-4E67-9EE2-A804D8E614DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86989EBE-988B-466B-9B6B-E66FCA27294C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26727,7 +26727,7 @@
         <xdr:cNvPr id="365" name="文字方塊 364">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95385AF-9730-4482-BD6B-CE91B6017ACE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06B8993C-8B49-40C4-B8B7-142AD3B8F60D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26825,7 +26825,7 @@
         <xdr:cNvPr id="366" name="文字方塊 365">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E9DD5E1-013C-4D04-80A5-6397D8186E35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8366DA5B-F2CF-4844-B4B8-96111812AE3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26923,7 +26923,7 @@
         <xdr:cNvPr id="367" name="文字方塊 366">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10F1E513-8ADB-44BC-94A2-D2CC7E7D3282}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570EF019-227C-48B2-8177-29C00EF41309}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27021,7 +27021,7 @@
         <xdr:cNvPr id="368" name="文字方塊 367">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA4CE84-644C-4522-A9A9-03C4882A7E52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001CBAE4-9B62-4E9F-99E0-C62B2C5F3CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27119,7 +27119,7 @@
         <xdr:cNvPr id="369" name="文字方塊 368">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE9DF5FF-7DE1-4414-9FD4-7A87632CEAF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF273094-ECEC-4BA0-B7EA-AFF70EB552F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27217,7 +27217,7 @@
         <xdr:cNvPr id="370" name="文字方塊 369">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBC244C-9D39-4C0E-BF05-E93C0A87552B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64913EDF-59D5-4788-91E3-EB8E761127B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28041,7 +28041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B393DFDC-6A71-4AFD-8C1F-30F0653F53DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AF4667-DE9B-4A09-BD98-2887C9435A22}">
   <dimension ref="A1:AP48"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A44" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>